<commit_message>
Added permutation importance in regression_model.py. Added description in house-prices-scheme-experiments.xlsx
</commit_message>
<xml_diff>
--- a/house-prices-scheme-experiments.xlsx
+++ b/house-prices-scheme-experiments.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gosha\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gosha\Desktop\Projects\Improvements-to-ML-algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3247E22-38FE-453C-A3E3-78FCC86ADE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708AD641-6537-4C82-83EB-179AD37C2193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{EC849CF7-2535-4AD3-8B1A-AE9429A52AE7}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>Combination of preprocessing methods</t>
   </si>
@@ -382,7 +382,13 @@
     <t>Hash Encoding + K-NN (3 neighbor)</t>
   </si>
   <si>
-    <t>Dataset: house-prices-advanced-regression-techniques. Missing values: 6965 / 115340, (6.039%)</t>
+    <t xml:space="preserve">Dataset: house-prices-advanced-regression-techniques. </t>
+  </si>
+  <si>
+    <t>X: [1460 rows x 79 columns] y: [1460 rows x 1 column]; Column type counts: {object: 43, int64: 33, float64: 3} Missing values: 6965 / 115340, (6.039%)</t>
+  </si>
+  <si>
+    <t>111 combinations of methods</t>
   </si>
 </sst>
 </file>
@@ -417,7 +423,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -425,11 +431,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -442,6 +485,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -761,7 +813,7 @@
   <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -772,9 +824,15 @@
     <col min="4" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="36" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:3" ht="54.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>116</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fixed datatype of output after K-NN
</commit_message>
<xml_diff>
--- a/house-prices-scheme-experiments.xlsx
+++ b/house-prices-scheme-experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gosha\Desktop\Projects\Improvements-to-ML-algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708AD641-6537-4C82-83EB-179AD37C2193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59180C30-328B-46E1-9BFA-101A500EA0DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{EC849CF7-2535-4AD3-8B1A-AE9429A52AE7}"/>
+    <workbookView xWindow="2232" yWindow="2184" windowWidth="17064" windowHeight="9468" xr2:uid="{EC849CF7-2535-4AD3-8B1A-AE9429A52AE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="125">
   <si>
     <t>Combination of preprocessing methods</t>
   </si>
@@ -389,6 +389,24 @@
   </si>
   <si>
     <t>111 combinations of methods</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>27582.549 (5511.916)</t>
+  </si>
+  <si>
+    <t>All data have benn discarded</t>
+  </si>
+  <si>
+    <t>28880.901 (6076.030)</t>
+  </si>
+  <si>
+    <t>27590.100 (5304.058)</t>
+  </si>
+  <si>
+    <t>29731.784 (5969.208)</t>
   </si>
 </sst>
 </file>
@@ -813,13 +831,13 @@
   <dimension ref="A1:C142"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.21875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="58.44140625" style="4" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="4"/>
   </cols>
@@ -853,15 +871,23 @@
       <c r="A4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
@@ -872,43 +898,67 @@
       <c r="A7" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
@@ -920,28 +970,36 @@
         <v>98</v>
       </c>
       <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="C14" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="C17" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
@@ -950,7 +1008,9 @@
       <c r="B18" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="3"/>
+      <c r="C18" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
@@ -962,21 +1022,27 @@
         <v>101</v>
       </c>
       <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="C22" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -988,21 +1054,27 @@
         <v>104</v>
       </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
@@ -1014,21 +1086,27 @@
         <v>107</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="C28" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
@@ -1040,21 +1118,27 @@
         <v>110</v>
       </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
@@ -1065,21 +1149,27 @@
         <v>113</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="C36" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="C37" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>115</v>
       </c>
       <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="C38" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
@@ -1192,21 +1282,27 @@
       <c r="A56" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B56" s="3"/>
+      <c r="B56" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C56" s="3"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B57" s="3"/>
+      <c r="B57" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B58" s="3"/>
+      <c r="B58" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -1218,21 +1314,27 @@
       <c r="A60" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B60" s="3"/>
+      <c r="B60" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C60" s="3"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B61" s="3"/>
+      <c r="B61" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C61" s="3"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B62" s="3"/>
+      <c r="B62" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C62" s="3"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -1244,21 +1346,27 @@
       <c r="A64" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B64" s="3"/>
+      <c r="B64" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C64" s="3"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B65" s="3"/>
+      <c r="B65" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C65" s="3"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="3"/>
+      <c r="B66" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C66" s="3"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -1270,21 +1378,27 @@
       <c r="A68" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B68" s="3"/>
+      <c r="B68" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C68" s="3"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B69" s="3"/>
+      <c r="B69" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C69" s="3"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B70" s="3"/>
+      <c r="B70" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="C70" s="3"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added configuration for 30 / 50 (2nd dataset) %
</commit_message>
<xml_diff>
--- a/house-prices-scheme-experiments.xlsx
+++ b/house-prices-scheme-experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gosha\Desktop\Projects\Improvements-to-ML-algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D44219-51C5-4630-BE6C-96545A156586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C83CC6-3C90-4EB6-8B20-79C6142E7382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{EC849CF7-2535-4AD3-8B1A-AE9429A52AE7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{EC849CF7-2535-4AD3-8B1A-AE9429A52AE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Original 6%" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="596">
   <si>
     <t>Combination of preprocessing methods</t>
   </si>
@@ -1839,12 +1839,15 @@
   <si>
     <t>0.0038258 (0.0008382)</t>
   </si>
+  <si>
+    <t>Missing values: 57741 / 115340 (50.062%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2324,11 +2327,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A13D3B5-F0CB-4832-A8C7-53C4A54DD8C9}">
   <dimension ref="A1:I142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="51" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="51" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="35.88671875" style="4" bestFit="1" customWidth="1"/>
@@ -2342,7 +2345,7 @@
     <col min="10" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="54">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -2356,12 +2359,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="36">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2375,7 +2378,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -2389,7 +2392,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2403,13 +2406,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -2423,7 +2426,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -2437,7 +2440,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -2451,7 +2454,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -2465,7 +2468,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -2493,13 +2496,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -2513,7 +2516,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -2527,7 +2530,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -2541,7 +2544,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -2555,7 +2558,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -2569,13 +2572,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -2589,7 +2592,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -2617,13 +2620,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -2637,7 +2640,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -2651,7 +2654,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -2665,13 +2668,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -2685,7 +2688,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -2713,13 +2716,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -2733,7 +2736,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -2747,7 +2750,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -2761,12 +2764,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -2780,7 +2783,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -2794,7 +2797,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -2808,13 +2811,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -2828,7 +2831,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -2842,7 +2845,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -2856,13 +2859,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -2876,7 +2879,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -2890,7 +2893,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -2904,12 +2907,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -2923,7 +2926,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -2937,7 +2940,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -2951,12 +2954,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -2970,7 +2973,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -2998,12 +3001,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -3031,7 +3034,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -3045,13 +3048,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -3065,7 +3068,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -3093,13 +3096,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -3113,7 +3116,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -3127,7 +3130,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -3141,13 +3144,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -3161,7 +3164,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -3175,7 +3178,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -3189,12 +3192,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -3208,7 +3211,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -3222,7 +3225,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -3236,7 +3239,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -3250,7 +3253,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -3264,7 +3267,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -3281,7 +3284,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -3307,7 +3310,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -3333,7 +3336,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -3347,7 +3350,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
@@ -3361,7 +3364,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -3375,11 +3378,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -3393,7 +3396,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -3407,7 +3410,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -3421,7 +3424,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -3435,7 +3438,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -3449,10 +3452,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -3466,7 +3469,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -3480,7 +3483,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -3494,7 +3497,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -3508,7 +3511,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -3522,7 +3525,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9">
       <c r="A95" s="2"/>
       <c r="F95" s="22" t="s">
         <v>304</v>
@@ -3537,7 +3540,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -3563,7 +3566,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -3589,7 +3592,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
@@ -3603,7 +3606,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -3617,7 +3620,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -3631,10 +3634,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -3648,7 +3651,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -3662,7 +3665,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -3676,7 +3679,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -3690,7 +3693,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -3704,10 +3707,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -3721,7 +3724,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -3735,7 +3738,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -3763,7 +3766,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -3777,7 +3780,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -3803,7 +3806,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -3829,7 +3832,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -3855,7 +3858,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -3869,7 +3872,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -3883,7 +3886,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -3897,7 +3900,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -3925,7 +3928,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -3939,7 +3942,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -3953,7 +3956,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -3967,7 +3970,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -3981,7 +3984,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
@@ -3995,7 +3998,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -4009,7 +4012,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -4023,7 +4026,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9">
       <c r="F131" s="22" t="s">
         <v>310</v>
       </c>
@@ -4037,7 +4040,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -4063,7 +4066,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9">
       <c r="A133" s="4" t="s">
         <v>80</v>
       </c>
@@ -4089,7 +4092,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -4103,7 +4106,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
@@ -4117,7 +4120,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -4131,7 +4134,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -4145,7 +4148,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -4159,7 +4162,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -4173,7 +4176,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -4187,7 +4190,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>
@@ -4215,7 +4218,7 @@
       <selection activeCell="B117" sqref="B117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="34.21875" style="4" bestFit="1" customWidth="1"/>
@@ -4228,7 +4231,7 @@
     <col min="10" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="54">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -4242,12 +4245,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="36">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4261,7 +4264,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -4275,7 +4278,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -4290,13 +4293,13 @@
       </c>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -4310,7 +4313,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -4324,7 +4327,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -4338,7 +4341,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -4352,7 +4355,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -4366,7 +4369,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -4380,13 +4383,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -4400,7 +4403,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -4414,7 +4417,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -4428,7 +4431,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -4442,7 +4445,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -4456,13 +4459,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -4476,7 +4479,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -4490,7 +4493,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -4504,13 +4507,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -4524,7 +4527,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -4538,7 +4541,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -4552,13 +4555,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -4572,7 +4575,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -4586,7 +4589,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -4600,13 +4603,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -4620,7 +4623,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -4634,7 +4637,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -4648,12 +4651,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -4667,7 +4670,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -4681,7 +4684,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -4695,13 +4698,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -4715,7 +4718,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -4729,7 +4732,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -4743,13 +4746,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -4763,7 +4766,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -4777,7 +4780,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -4791,12 +4794,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -4810,7 +4813,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -4824,7 +4827,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -4838,12 +4841,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4857,7 +4860,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -4871,7 +4874,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -4885,12 +4888,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -4904,7 +4907,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -4918,7 +4921,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -4932,13 +4935,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -4952,7 +4955,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -4966,7 +4969,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -4980,13 +4983,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -5000,7 +5003,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -5014,7 +5017,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -5028,13 +5031,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -5048,7 +5051,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -5062,7 +5065,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -5076,12 +5079,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -5095,7 +5098,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -5109,7 +5112,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -5123,7 +5126,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -5137,7 +5140,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -5151,12 +5154,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -5170,7 +5173,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -5184,7 +5187,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -5198,7 +5201,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
@@ -5212,7 +5215,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -5226,11 +5229,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -5244,7 +5247,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -5258,7 +5261,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -5272,7 +5275,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -5286,7 +5289,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -5300,10 +5303,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -5317,7 +5320,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -5331,7 +5334,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -5345,7 +5348,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -5359,7 +5362,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -5373,10 +5376,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -5390,7 +5393,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -5404,7 +5407,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
@@ -5418,7 +5421,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -5432,7 +5435,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -5446,10 +5449,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -5463,7 +5466,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -5477,7 +5480,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -5491,7 +5494,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -5505,7 +5508,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -5519,10 +5522,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -5536,7 +5539,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -5550,7 +5553,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -5564,7 +5567,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -5578,7 +5581,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -5592,7 +5595,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -5606,7 +5609,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -5620,7 +5623,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -5634,7 +5637,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -5648,7 +5651,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -5662,7 +5665,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -5676,7 +5679,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -5690,7 +5693,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -5704,7 +5707,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -5718,7 +5721,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -5732,7 +5735,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -5746,7 +5749,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -5760,7 +5763,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
@@ -5774,7 +5777,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -5788,7 +5791,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -5802,7 +5805,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -5816,7 +5819,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
         <v>423</v>
       </c>
@@ -5830,7 +5833,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -5844,7 +5847,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
@@ -5858,7 +5861,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -5872,7 +5875,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -5886,7 +5889,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -5900,7 +5903,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -5914,7 +5917,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -5928,7 +5931,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>
@@ -5952,11 +5955,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF4B17E-1BBF-4C2E-9D6B-BC1E5266428F}">
   <dimension ref="A1:D142"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="27" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="S55" sqref="S55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="34.21875" style="4" bestFit="1" customWidth="1"/>
@@ -5966,12 +5969,12 @@
     <col min="6" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="54">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>274</v>
+        <v>595</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>146</v>
@@ -5980,12 +5983,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="36">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5999,7 +6002,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -6013,7 +6016,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -6027,13 +6030,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -6047,7 +6050,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -6061,7 +6064,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -6075,7 +6078,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -6089,7 +6092,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -6103,7 +6106,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -6117,13 +6120,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -6137,7 +6140,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -6151,7 +6154,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -6165,7 +6168,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -6179,7 +6182,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -6193,13 +6196,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -6213,7 +6216,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -6227,7 +6230,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -6241,13 +6244,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -6261,7 +6264,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -6275,7 +6278,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -6289,13 +6292,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -6309,7 +6312,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -6323,7 +6326,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -6337,13 +6340,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -6357,7 +6360,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -6371,7 +6374,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -6385,12 +6388,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -6404,7 +6407,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -6418,7 +6421,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -6432,13 +6435,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -6452,7 +6455,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -6466,7 +6469,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -6480,13 +6483,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -6500,7 +6503,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -6514,7 +6517,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -6528,12 +6531,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -6547,7 +6550,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -6561,7 +6564,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -6575,12 +6578,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -6594,7 +6597,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -6608,7 +6611,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -6622,12 +6625,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -6641,7 +6644,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -6655,7 +6658,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -6669,13 +6672,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -6689,7 +6692,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -6703,7 +6706,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -6717,13 +6720,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -6737,7 +6740,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -6751,7 +6754,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -6765,13 +6768,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -6785,7 +6788,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -6799,7 +6802,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -6813,12 +6816,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -6832,7 +6835,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:4">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -6846,7 +6849,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -6860,7 +6863,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -6874,7 +6877,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:4">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -6888,12 +6891,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -6907,7 +6910,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -6921,7 +6924,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -6935,7 +6938,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
@@ -6949,7 +6952,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -6963,11 +6966,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -6981,7 +6984,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -6995,7 +6998,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -7009,7 +7012,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -7023,7 +7026,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -7037,10 +7040,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -7054,7 +7057,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -7068,7 +7071,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -7082,7 +7085,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -7096,7 +7099,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -7110,10 +7113,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -7127,7 +7130,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -7141,7 +7144,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
@@ -7155,7 +7158,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -7169,7 +7172,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -7183,10 +7186,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -7200,7 +7203,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -7214,7 +7217,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -7228,7 +7231,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -7242,7 +7245,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -7256,10 +7259,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -7273,7 +7276,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -7287,7 +7290,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -7301,7 +7304,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -7315,7 +7318,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -7329,7 +7332,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -7343,7 +7346,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -7357,7 +7360,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -7371,7 +7374,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -7385,7 +7388,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -7399,7 +7402,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -7413,7 +7416,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -7427,7 +7430,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -7441,7 +7444,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -7455,7 +7458,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -7469,7 +7472,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -7483,7 +7486,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -7497,7 +7500,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
@@ -7511,7 +7514,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -7525,7 +7528,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -7539,7 +7542,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -7553,7 +7556,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
         <v>80</v>
       </c>
@@ -7567,7 +7570,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -7581,7 +7584,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
@@ -7595,7 +7598,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -7609,7 +7612,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -7623,7 +7626,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -7637,7 +7640,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -7651,7 +7654,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -7665,7 +7668,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Added best models combination
</commit_message>
<xml_diff>
--- a/house-prices-scheme-experiments.xlsx
+++ b/house-prices-scheme-experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gosha\Desktop\Projects\Improvements-to-ML-algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C83CC6-3C90-4EB6-8B20-79C6142E7382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1321ED-9C61-4547-91D9-F9777B0A5301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{EC849CF7-2535-4AD3-8B1A-AE9429A52AE7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1411" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1468" uniqueCount="611">
   <si>
     <t>Combination of preprocessing methods</t>
   </si>
@@ -1842,12 +1842,57 @@
   <si>
     <t>Missing values: 57741 / 115340 (50.062%)</t>
   </si>
+  <si>
+    <t>6% of missing data</t>
+  </si>
+  <si>
+    <t>The importance of the anomaly indicator</t>
+  </si>
+  <si>
+    <t>1. Default model</t>
+  </si>
+  <si>
+    <t>2. Elliptic Envelope (Target Encoding + Median imputation)</t>
+  </si>
+  <si>
+    <t>6. (Best) MICE</t>
+  </si>
+  <si>
+    <t>3. One-Class SVM (Target Encoding + Median imputation)</t>
+  </si>
+  <si>
+    <t>4. Isolation Forest (Target Encoding + Mode imputation)</t>
+  </si>
+  <si>
+    <t>5. LocalOutlierFactor( Target Encoding + K-NN)</t>
+  </si>
+  <si>
+    <t>30% of missing data</t>
+  </si>
+  <si>
+    <t>2. Elliptic Envelope (Target Encoding + MICE)</t>
+  </si>
+  <si>
+    <t>3. One-Class SVM(Target Encoding + MICE)</t>
+  </si>
+  <si>
+    <t>4. Isolation Forest (Target Encoding + MICE)</t>
+  </si>
+  <si>
+    <t>5. LocalOutlierFactor (Target Encoding + MICE)</t>
+  </si>
+  <si>
+    <t>50% of missing data</t>
+  </si>
+  <si>
+    <t>3. (Best) One-Class SVM(Target Encoding + MICE)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1890,6 +1935,12 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
       <family val="1"/>
     </font>
   </fonts>
@@ -1946,7 +1997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2011,6 +2062,22 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2325,13 +2392,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A13D3B5-F0CB-4832-A8C7-53C4A54DD8C9}">
-  <dimension ref="A1:I142"/>
+  <dimension ref="A1:O142"/>
   <sheetViews>
-    <sheetView zoomScale="51" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A68" zoomScale="64" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="M77" sqref="M77:O83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="35.88671875" style="4" bestFit="1" customWidth="1"/>
@@ -2342,10 +2409,14 @@
     <col min="7" max="7" width="29.6640625" style="4" customWidth="1"/>
     <col min="8" max="8" width="29.88671875" style="4" customWidth="1"/>
     <col min="9" max="9" width="17" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="4"/>
+    <col min="10" max="12" width="8.88671875" style="4"/>
+    <col min="13" max="13" width="63.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.77734375" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="54">
+    <row r="1" spans="1:4" ht="54" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -2359,12 +2430,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36">
+    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2378,7 +2449,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -2392,7 +2463,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2406,13 +2477,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -2426,7 +2497,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -2440,7 +2511,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -2454,7 +2525,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -2468,7 +2539,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -2482,7 +2553,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -2496,13 +2567,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -2516,7 +2587,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -2530,7 +2601,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -2544,7 +2615,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -2558,7 +2629,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -2572,13 +2643,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -2592,7 +2663,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -2606,7 +2677,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -2620,13 +2691,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -2640,7 +2711,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -2654,7 +2725,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -2668,13 +2739,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -2688,7 +2759,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -2702,7 +2773,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -2716,13 +2787,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -2736,7 +2807,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -2750,7 +2821,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -2764,12 +2835,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -2783,7 +2854,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -2797,7 +2868,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -2811,13 +2882,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -2831,7 +2902,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -2845,7 +2916,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -2859,13 +2930,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -2879,7 +2950,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -2893,7 +2964,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -2907,12 +2978,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -2926,7 +2997,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -2940,7 +3011,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -2954,12 +3025,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -2973,7 +3044,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -2987,7 +3058,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -3001,12 +3072,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -3020,7 +3091,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -3034,7 +3105,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -3048,13 +3119,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -3068,7 +3139,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -3082,7 +3153,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -3096,13 +3167,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -3116,7 +3187,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:9">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -3130,7 +3201,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:9">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -3144,13 +3215,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:9">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:9">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -3164,7 +3235,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:9">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -3178,7 +3249,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:9">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -3192,12 +3263,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:9">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:9">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -3211,7 +3282,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:9">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -3225,7 +3296,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:9">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -3239,7 +3310,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:9">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -3253,7 +3324,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:9">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -3267,7 +3338,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:9">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -3283,8 +3354,17 @@
       <c r="I77" s="16" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="78" spans="1:9">
+      <c r="M77" s="30" t="s">
+        <v>596</v>
+      </c>
+      <c r="N77" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="O77" s="30" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -3309,8 +3389,17 @@
       <c r="I78" s="17">
         <v>113</v>
       </c>
-    </row>
-    <row r="79" spans="1:9">
+      <c r="M78" s="29" t="s">
+        <v>598</v>
+      </c>
+      <c r="N78" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="O78" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -3335,8 +3424,17 @@
       <c r="I79" s="16">
         <v>146</v>
       </c>
-    </row>
-    <row r="80" spans="1:9">
+      <c r="M79" s="29" t="s">
+        <v>599</v>
+      </c>
+      <c r="N79" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="O79" s="29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -3349,8 +3447,17 @@
       <c r="D80" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="81" spans="1:9">
+      <c r="M80" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="N80" s="32" t="s">
+        <v>189</v>
+      </c>
+      <c r="O80" s="32" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
@@ -3363,8 +3470,17 @@
       <c r="D81" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="82" spans="1:9">
+      <c r="M81" s="32" t="s">
+        <v>602</v>
+      </c>
+      <c r="N81" s="32" t="s">
+        <v>226</v>
+      </c>
+      <c r="O81" s="32" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -3377,12 +3493,30 @@
       <c r="D82" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="83" spans="1:9">
+      <c r="M82" s="32" t="s">
+        <v>603</v>
+      </c>
+      <c r="N82" s="32" t="s">
+        <v>261</v>
+      </c>
+      <c r="O82" s="32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
-    </row>
-    <row r="84" spans="1:9">
+      <c r="M83" s="29" t="s">
+        <v>600</v>
+      </c>
+      <c r="N83" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="O83" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -3395,8 +3529,11 @@
       <c r="D84" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="85" spans="1:9">
+      <c r="M84" s="28"/>
+      <c r="N84" s="28"/>
+      <c r="O84" s="28"/>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -3409,8 +3546,10 @@
       <c r="D85" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="86" spans="1:9">
+      <c r="N85" s="28"/>
+      <c r="O85" s="28"/>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -3423,8 +3562,10 @@
       <c r="D86" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="87" spans="1:9">
+      <c r="N86" s="28"/>
+      <c r="O86" s="28"/>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -3437,8 +3578,10 @@
       <c r="D87" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="88" spans="1:9">
+      <c r="N87" s="28"/>
+      <c r="O87" s="28"/>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -3451,11 +3594,14 @@
       <c r="D88" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="89" spans="1:9">
+      <c r="N88" s="28"/>
+      <c r="O88" s="28"/>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
-    </row>
-    <row r="90" spans="1:9">
+      <c r="O89" s="28"/>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -3468,8 +3614,10 @@
       <c r="D90" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="91" spans="1:9">
+      <c r="N90" s="28"/>
+      <c r="O90" s="28"/>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -3483,7 +3631,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:9">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -3497,7 +3645,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:9">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -3511,7 +3659,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="94" spans="1:9">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -3525,7 +3673,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:9">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="F95" s="22" t="s">
         <v>304</v>
@@ -3540,7 +3688,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="96" spans="1:9">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -3566,7 +3714,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="97" spans="1:9">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -3592,7 +3740,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="98" spans="1:9">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
@@ -3606,7 +3754,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="99" spans="1:9">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -3620,7 +3768,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:9">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -3634,10 +3782,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:9">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:9">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -3651,7 +3799,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="103" spans="1:9">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -3665,7 +3813,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:9">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -3679,7 +3827,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:9">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -3693,7 +3841,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="106" spans="1:9">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -3707,10 +3855,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="107" spans="1:9">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:9">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -3724,7 +3872,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:9">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -3738,7 +3886,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:9">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -3752,7 +3900,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:9">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -3766,7 +3914,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -3780,7 +3928,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -3806,7 +3954,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="115" spans="1:9">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -3832,7 +3980,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="1:9">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -3858,7 +4006,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:9">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -3872,7 +4020,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:9">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -3886,7 +4034,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="120" spans="1:9">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -3900,7 +4048,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -3914,7 +4062,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="122" spans="1:9">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -3928,7 +4076,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="123" spans="1:9">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -3942,7 +4090,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="124" spans="1:9">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -3956,7 +4104,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:9">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -3970,7 +4118,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="127" spans="1:9">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -3984,7 +4132,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="128" spans="1:9">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
@@ -3998,7 +4146,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:9">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -4012,7 +4160,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="130" spans="1:9">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -4026,7 +4174,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="F131" s="22" t="s">
         <v>310</v>
       </c>
@@ -4040,7 +4188,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="132" spans="1:9">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -4066,7 +4214,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="133" spans="1:9">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>80</v>
       </c>
@@ -4092,7 +4240,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="134" spans="1:9">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -4106,7 +4254,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="135" spans="1:9">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
@@ -4120,7 +4268,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="136" spans="1:9">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -4134,7 +4282,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="138" spans="1:9">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -4148,7 +4296,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="139" spans="1:9">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -4162,7 +4310,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="140" spans="1:9">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -4176,7 +4324,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="141" spans="1:9">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -4190,7 +4338,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="142" spans="1:9">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>
@@ -4212,13 +4360,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A8515C-8539-4E5E-AB27-D793F52CD44C}">
-  <dimension ref="A1:H142"/>
+  <dimension ref="A1:J142"/>
   <sheetViews>
-    <sheetView zoomScale="28" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView topLeftCell="B52" zoomScale="62" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72:J77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="34.21875" style="4" bestFit="1" customWidth="1"/>
@@ -4226,12 +4374,13 @@
     <col min="4" max="4" width="24.88671875" style="4" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" style="4" customWidth="1"/>
     <col min="6" max="7" width="8.88671875" style="4"/>
-    <col min="8" max="8" width="27.33203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="74.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="45.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="54">
+    <row r="1" spans="1:8" ht="54" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -4245,12 +4394,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="36">
+    <row r="3" spans="1:8" ht="36" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4264,7 +4413,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -4278,7 +4427,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -4293,13 +4442,13 @@
       </c>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -4313,7 +4462,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -4327,7 +4476,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -4341,7 +4490,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -4355,7 +4504,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -4369,7 +4518,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -4383,13 +4532,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -4403,7 +4552,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -4417,7 +4566,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -4431,7 +4580,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -4445,7 +4594,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -4459,13 +4608,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -4479,7 +4628,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -4493,7 +4642,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -4507,13 +4656,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -4527,7 +4676,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -4541,7 +4690,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -4555,13 +4704,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -4575,7 +4724,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -4589,7 +4738,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -4603,13 +4752,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -4623,7 +4772,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -4637,7 +4786,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -4651,12 +4800,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -4670,7 +4819,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -4684,7 +4833,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -4698,13 +4847,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -4718,7 +4867,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -4732,7 +4881,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -4746,13 +4895,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -4766,7 +4915,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -4780,7 +4929,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -4794,12 +4943,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -4813,7 +4962,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -4827,7 +4976,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -4841,12 +4990,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -4860,7 +5009,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -4874,7 +5023,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -4888,12 +5037,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -4907,7 +5056,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -4921,7 +5070,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -4935,13 +5084,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -4955,7 +5104,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -4969,7 +5118,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -4983,13 +5132,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -5003,7 +5152,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -5017,7 +5166,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -5031,13 +5180,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -5051,7 +5200,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -5065,7 +5214,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -5079,12 +5228,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -5097,8 +5246,17 @@
       <c r="D72" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="H72" s="30" t="s">
+        <v>604</v>
+      </c>
+      <c r="I72" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J72" s="30" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -5111,8 +5269,17 @@
       <c r="D73" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="H73" s="29" t="s">
+        <v>598</v>
+      </c>
+      <c r="I73" s="29" t="s">
+        <v>275</v>
+      </c>
+      <c r="J73" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -5125,8 +5292,17 @@
       <c r="D74" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="H74" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -5139,8 +5315,17 @@
       <c r="D75" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="H75" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -5153,13 +5338,31 @@
       <c r="D76" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="H76" s="4" t="s">
+        <v>607</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="H77" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -5172,22 +5375,25 @@
       <c r="D78" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="H78" s="29"/>
+      <c r="I78" s="29"/>
+      <c r="J78" s="29"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="C79" s="3" t="s">
+      <c r="C79" s="8" t="s">
         <v>326</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -5201,11 +5407,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="8" t="s">
         <v>329</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -5215,7 +5421,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -5229,11 +5435,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -5247,7 +5453,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -5261,7 +5467,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -5275,7 +5481,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -5289,7 +5495,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -5303,10 +5509,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -5320,7 +5526,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -5334,7 +5540,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -5348,7 +5554,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -5362,7 +5568,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -5376,10 +5582,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -5393,39 +5599,39 @@
         <v>175</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B97" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C97" s="4" t="s">
+      <c r="C97" s="7" t="s">
         <v>356</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B98" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="C98" s="11" t="s">
+      <c r="C98" s="4" t="s">
         <v>359</v>
       </c>
       <c r="D98" s="4" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B99" s="4" t="s">
+      <c r="B99" s="7" t="s">
         <v>360</v>
       </c>
       <c r="C99" s="4" t="s">
@@ -5435,7 +5641,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -5449,10 +5655,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -5466,7 +5672,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -5480,7 +5686,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -5494,7 +5700,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -5508,7 +5714,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -5522,10 +5728,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -5539,7 +5745,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -5553,7 +5759,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -5567,7 +5773,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -5581,7 +5787,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -5595,7 +5801,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -5609,7 +5815,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -5623,7 +5829,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -5637,7 +5843,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -5651,7 +5857,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -5665,7 +5871,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -5679,7 +5885,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -5693,7 +5899,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -5707,7 +5913,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -5721,7 +5927,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -5735,7 +5941,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -5749,7 +5955,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -5763,21 +5969,21 @@
         <v>407</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B128" s="4" t="s">
         <v>410</v>
       </c>
-      <c r="C128" s="4" t="s">
+      <c r="C128" s="7" t="s">
         <v>411</v>
       </c>
       <c r="D128" s="4" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -5791,7 +5997,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -5805,7 +6011,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -5819,7 +6025,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>423</v>
       </c>
@@ -5833,7 +6039,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -5847,11 +6053,11 @@
         <v>427</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="7" t="s">
         <v>416</v>
       </c>
       <c r="C135" s="4" t="s">
@@ -5861,7 +6067,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -5875,7 +6081,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -5889,7 +6095,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -5903,7 +6109,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -5917,7 +6123,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -5931,7 +6137,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>
@@ -5953,23 +6159,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF4B17E-1BBF-4C2E-9D6B-BC1E5266428F}">
-  <dimension ref="A1:D142"/>
+  <dimension ref="A1:M142"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="S55" sqref="S55"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="34.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.77734375" style="4" customWidth="1"/>
     <col min="4" max="4" width="24.88671875" style="4" customWidth="1"/>
     <col min="5" max="5" width="14.88671875" style="4" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="4"/>
+    <col min="6" max="10" width="8.88671875" style="4"/>
+    <col min="11" max="11" width="58.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="48.109375" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="54">
+    <row r="1" spans="1:4" ht="54" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -5983,12 +6193,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36">
+    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6002,7 +6212,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -6016,7 +6226,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -6030,13 +6240,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -6050,7 +6260,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -6064,7 +6274,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -6078,7 +6288,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -6092,7 +6302,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -6106,7 +6316,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -6120,13 +6330,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -6140,7 +6350,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -6154,7 +6364,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -6168,7 +6378,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -6182,7 +6392,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -6196,13 +6406,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -6216,7 +6426,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -6230,7 +6440,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -6244,13 +6454,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -6264,7 +6474,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -6278,7 +6488,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -6292,13 +6502,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -6312,7 +6522,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -6326,7 +6536,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -6340,13 +6550,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -6360,7 +6570,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -6374,7 +6584,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -6388,12 +6598,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -6407,7 +6617,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -6421,7 +6631,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -6435,13 +6645,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -6455,7 +6665,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -6469,7 +6679,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -6483,13 +6693,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -6503,7 +6713,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -6517,7 +6727,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -6531,12 +6741,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -6550,7 +6760,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -6564,7 +6774,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -6578,12 +6788,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -6597,7 +6807,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -6611,7 +6821,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -6625,12 +6835,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -6644,7 +6854,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -6658,7 +6868,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -6672,13 +6882,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -6692,7 +6902,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -6706,7 +6916,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -6720,13 +6930,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -6740,7 +6950,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -6754,7 +6964,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -6768,13 +6978,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -6788,7 +6998,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -6802,7 +7012,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -6816,12 +7026,21 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="K71" s="29" t="s">
+        <v>609</v>
+      </c>
+      <c r="L71" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="M71" s="30" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -6834,8 +7053,17 @@
       <c r="D72" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="K72" s="29" t="s">
+        <v>598</v>
+      </c>
+      <c r="L72" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="M72" s="29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -6848,8 +7076,17 @@
       <c r="D73" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="K73" s="33" t="s">
+        <v>605</v>
+      </c>
+      <c r="L73" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="M73" s="3" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -6862,8 +7099,17 @@
       <c r="D74" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="K74" s="33" t="s">
+        <v>610</v>
+      </c>
+      <c r="L74" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="M74" s="4" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -6876,8 +7122,17 @@
       <c r="D75" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="K75" s="31" t="s">
+        <v>607</v>
+      </c>
+      <c r="L75" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="M75" s="4" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -6890,13 +7145,22 @@
       <c r="D76" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="K76" s="31" t="s">
+        <v>608</v>
+      </c>
+      <c r="L76" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -6910,7 +7174,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -6924,7 +7188,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -6938,7 +7202,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
@@ -6952,7 +7216,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -6966,11 +7230,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -6984,7 +7248,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -6998,7 +7262,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -7012,7 +7276,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -7026,7 +7290,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -7040,10 +7304,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -7057,7 +7321,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -7071,7 +7335,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -7085,7 +7349,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -7099,7 +7363,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -7113,10 +7377,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -7130,7 +7394,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -7144,7 +7408,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
@@ -7158,7 +7422,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -7172,7 +7436,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -7186,10 +7450,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -7203,7 +7467,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -7217,7 +7481,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -7231,7 +7495,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -7245,7 +7509,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -7259,10 +7523,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -7276,7 +7540,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -7290,7 +7554,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -7304,7 +7568,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -7318,7 +7582,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -7332,7 +7596,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:4">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -7346,7 +7610,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:4">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -7360,7 +7624,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:4">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -7374,7 +7638,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:4">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -7388,7 +7652,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:4">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -7402,7 +7666,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:4">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -7416,7 +7680,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="121" spans="1:4">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -7430,7 +7694,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -7444,7 +7708,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="123" spans="1:4">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -7458,7 +7722,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="124" spans="1:4">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -7472,7 +7736,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:4">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -7486,7 +7750,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -7500,7 +7764,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="128" spans="1:4">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
@@ -7514,7 +7778,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -7528,7 +7792,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -7542,7 +7806,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -7556,7 +7820,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="4" t="s">
         <v>80</v>
       </c>
@@ -7570,7 +7834,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -7584,11 +7848,11 @@
         <v>576</v>
       </c>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B135" s="4" t="s">
+      <c r="B135" s="7" t="s">
         <v>579</v>
       </c>
       <c r="C135" s="4" t="s">
@@ -7598,7 +7862,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -7612,7 +7876,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -7626,7 +7890,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -7640,7 +7904,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -7654,7 +7918,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -7668,7 +7932,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Add MAE, R2 metrics
</commit_message>
<xml_diff>
--- a/house-prices-scheme-experiments.xlsx
+++ b/house-prices-scheme-experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gosha\Desktop\Projects\Improvements-to-ML-algorithms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F968F233-48D8-4443-A5A2-029583C90B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55AA7711-E2F0-4E0F-90DC-EE02A9D235C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{EC849CF7-2535-4AD3-8B1A-AE9429A52AE7}"/>
+    <workbookView xWindow="5736" yWindow="0" windowWidth="17064" windowHeight="9468" xr2:uid="{EC849CF7-2535-4AD3-8B1A-AE9429A52AE7}"/>
   </bookViews>
   <sheets>
     <sheet name="Original 6%" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1502" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="615">
   <si>
     <t>Combination of preprocessing methods</t>
   </si>
@@ -1888,9 +1888,6 @@
     <t>3. (Best) One-Class SVM(Target Encoding + MICE)</t>
   </si>
   <si>
-    <t>Best</t>
-  </si>
-  <si>
     <t>(Old) One-Hot Encoding (nan has become a feature of *_nan)</t>
   </si>
   <si>
@@ -1907,7 +1904,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2012,7 +2009,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2088,22 +2085,45 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2421,11 +2441,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A13D3B5-F0CB-4832-A8C7-53C4A54DD8C9}">
   <dimension ref="A1:O194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="61" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I145" sqref="I145"/>
+    <sheetView tabSelected="1" topLeftCell="D122" zoomScale="48" zoomScaleNormal="25" workbookViewId="0">
+      <selection activeCell="G147" sqref="G147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="35.88671875" style="4" bestFit="1" customWidth="1"/>
@@ -2437,13 +2457,13 @@
     <col min="8" max="8" width="29.88671875" style="4" customWidth="1"/>
     <col min="9" max="9" width="17" style="4" customWidth="1"/>
     <col min="10" max="12" width="8.88671875" style="4"/>
-    <col min="13" max="13" width="63.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.77734375" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="40.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="69.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.77734375" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="54">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -2457,12 +2477,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="36">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2476,7 +2496,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -2490,7 +2510,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -2504,13 +2524,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -2524,7 +2544,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -2538,7 +2558,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -2552,7 +2572,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -2566,7 +2586,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -2580,7 +2600,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -2594,13 +2614,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -2614,7 +2634,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -2628,7 +2648,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -2642,7 +2662,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -2656,7 +2676,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -2670,13 +2690,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -2690,7 +2710,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -2704,7 +2724,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -2718,13 +2738,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -2738,7 +2758,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -2752,7 +2772,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -2766,13 +2786,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -2786,7 +2806,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -2800,7 +2820,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -2814,13 +2834,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -2834,7 +2854,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -2848,7 +2868,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -2862,12 +2882,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -2881,7 +2901,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -2895,7 +2915,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -2909,13 +2929,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -2929,7 +2949,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -2943,7 +2963,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -2957,13 +2977,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -2977,7 +2997,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -2991,7 +3011,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -3005,12 +3025,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -3024,7 +3044,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -3038,7 +3058,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -3052,12 +3072,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -3071,7 +3091,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -3085,7 +3105,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -3099,12 +3119,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -3118,7 +3138,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -3132,7 +3152,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -3146,13 +3166,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -3166,7 +3186,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -3180,7 +3200,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -3194,13 +3214,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -3214,7 +3234,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:15">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -3228,7 +3248,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:15">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -3242,13 +3262,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:15">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:15">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -3262,7 +3282,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:15">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -3276,7 +3296,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:15">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -3290,12 +3310,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:15">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:15">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -3309,7 +3329,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:15">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -3323,7 +3343,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:15">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -3337,7 +3357,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:15">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -3351,7 +3371,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:15">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -3364,11 +3384,8 @@
       <c r="D76" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="M76" s="4" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:15">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -3384,17 +3401,17 @@
       <c r="I77" s="16" t="s">
         <v>301</v>
       </c>
-      <c r="M77" s="30" t="s">
+      <c r="M77" s="36" t="s">
         <v>596</v>
       </c>
-      <c r="N77" s="30" t="s">
+      <c r="N77" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="O77" s="30" t="s">
+      <c r="O77" s="36" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:15">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -3419,17 +3436,17 @@
       <c r="I78" s="17">
         <v>113</v>
       </c>
-      <c r="M78" s="29" t="s">
+      <c r="M78" s="37" t="s">
         <v>598</v>
       </c>
-      <c r="N78" s="29" t="s">
+      <c r="N78" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="O78" s="29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O78" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -3454,17 +3471,17 @@
       <c r="I79" s="16">
         <v>146</v>
       </c>
-      <c r="M79" s="29" t="s">
+      <c r="M79" s="37" t="s">
         <v>599</v>
       </c>
-      <c r="N79" s="29" t="s">
+      <c r="N79" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="O79" s="29" t="s">
+      <c r="O79" s="36" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:15">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -3477,17 +3494,17 @@
       <c r="D80" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="M80" s="2" t="s">
+      <c r="M80" s="38" t="s">
         <v>601</v>
       </c>
-      <c r="N80" s="32" t="s">
+      <c r="N80" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="O80" s="32" t="s">
+      <c r="O80" s="42" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:15">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
@@ -3500,17 +3517,17 @@
       <c r="D81" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="M81" s="32" t="s">
+      <c r="M81" s="39" t="s">
         <v>602</v>
       </c>
-      <c r="N81" s="32" t="s">
+      <c r="N81" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="O81" s="32" t="s">
+      <c r="O81" s="42" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:15">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -3523,30 +3540,30 @@
       <c r="D82" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="M82" s="32" t="s">
+      <c r="M82" s="39" t="s">
         <v>603</v>
       </c>
-      <c r="N82" s="32" t="s">
+      <c r="N82" s="42" t="s">
         <v>261</v>
       </c>
-      <c r="O82" s="32" t="s">
+      <c r="O82" s="42" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:15">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
-      <c r="M83" s="29" t="s">
+      <c r="M83" s="37" t="s">
         <v>600</v>
       </c>
-      <c r="N83" s="29" t="s">
+      <c r="N83" s="36" t="s">
         <v>123</v>
       </c>
-      <c r="O83" s="29" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O83" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -3560,10 +3577,10 @@
         <v>144</v>
       </c>
       <c r="M84" s="28"/>
-      <c r="N84" s="28"/>
-      <c r="O84" s="28"/>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N84" s="43"/>
+      <c r="O84" s="43"/>
+    </row>
+    <row r="85" spans="1:15">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -3576,10 +3593,17 @@
       <c r="D85" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="N85" s="28"/>
-      <c r="O85" s="28"/>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M85" s="36" t="s">
+        <v>604</v>
+      </c>
+      <c r="N85" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="O85" s="36" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -3592,10 +3616,17 @@
       <c r="D86" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="N86" s="28"/>
-      <c r="O86" s="28"/>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M86" s="37" t="s">
+        <v>598</v>
+      </c>
+      <c r="N86" s="36" t="s">
+        <v>275</v>
+      </c>
+      <c r="O86" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -3608,10 +3639,17 @@
       <c r="D87" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="N87" s="28"/>
-      <c r="O87" s="28"/>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M87" s="38" t="s">
+        <v>605</v>
+      </c>
+      <c r="N87" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="O87" s="44" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -3624,14 +3662,29 @@
       <c r="D88" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="N88" s="28"/>
-      <c r="O88" s="28"/>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M88" s="38" t="s">
+        <v>606</v>
+      </c>
+      <c r="N88" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="O88" s="42" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
       <c r="A89" s="2"/>
-      <c r="O89" s="28"/>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M89" s="35" t="s">
+        <v>607</v>
+      </c>
+      <c r="N89" s="42" t="s">
+        <v>390</v>
+      </c>
+      <c r="O89" s="42" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -3644,10 +3697,17 @@
       <c r="D90" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="N90" s="28"/>
-      <c r="O90" s="28"/>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M90" s="35" t="s">
+        <v>608</v>
+      </c>
+      <c r="N90" s="42" t="s">
+        <v>416</v>
+      </c>
+      <c r="O90" s="42" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -3660,8 +3720,10 @@
       <c r="D91" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N91" s="45"/>
+      <c r="O91" s="45"/>
+    </row>
+    <row r="92" spans="1:15">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -3674,8 +3736,17 @@
       <c r="D92" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M92" s="37" t="s">
+        <v>609</v>
+      </c>
+      <c r="N92" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="O92" s="36" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="93" spans="1:15">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -3688,8 +3759,17 @@
       <c r="D93" s="4" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M93" s="37" t="s">
+        <v>598</v>
+      </c>
+      <c r="N93" s="44" t="s">
+        <v>445</v>
+      </c>
+      <c r="O93" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="94" spans="1:15">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -3702,8 +3782,17 @@
       <c r="D94" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M94" s="40" t="s">
+        <v>605</v>
+      </c>
+      <c r="N94" s="44" t="s">
+        <v>485</v>
+      </c>
+      <c r="O94" s="44" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
       <c r="A95" s="2"/>
       <c r="F95" s="22" t="s">
         <v>304</v>
@@ -3717,8 +3806,17 @@
       <c r="I95" s="16" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="M95" s="40" t="s">
+        <v>610</v>
+      </c>
+      <c r="N95" s="42" t="s">
+        <v>514</v>
+      </c>
+      <c r="O95" s="42" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -3743,8 +3841,17 @@
       <c r="I96" s="17">
         <v>560</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M96" s="41" t="s">
+        <v>607</v>
+      </c>
+      <c r="N96" s="42" t="s">
+        <v>544</v>
+      </c>
+      <c r="O96" s="42" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -3769,8 +3876,17 @@
       <c r="I97" s="15">
         <v>730</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="M97" s="41" t="s">
+        <v>608</v>
+      </c>
+      <c r="N97" s="42" t="s">
+        <v>579</v>
+      </c>
+      <c r="O97" s="42" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
@@ -3784,7 +3900,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:15">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -3798,7 +3914,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:15">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -3812,10 +3928,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:15">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:15">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -3829,7 +3945,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:15">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -3843,7 +3959,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:15">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -3857,7 +3973,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:15">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -3871,7 +3987,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:15">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -3885,10 +4001,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:15">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:15">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -3902,7 +4018,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:15">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -3916,7 +4032,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:15">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -3930,7 +4046,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:15">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -3944,7 +4060,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:15">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -3958,7 +4074,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -3984,7 +4100,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -4010,7 +4126,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -4036,7 +4152,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -4050,7 +4166,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -4064,7 +4180,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -4078,7 +4194,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -4092,7 +4208,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -4106,7 +4222,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -4120,7 +4236,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -4134,7 +4250,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -4148,7 +4264,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -4162,7 +4278,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
@@ -4176,7 +4292,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -4190,7 +4306,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -4204,7 +4320,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9">
       <c r="F131" s="22" t="s">
         <v>310</v>
       </c>
@@ -4218,7 +4334,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -4244,7 +4360,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9">
       <c r="A133" s="4" t="s">
         <v>80</v>
       </c>
@@ -4270,7 +4386,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -4284,7 +4400,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
@@ -4298,7 +4414,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -4312,7 +4428,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -4326,7 +4442,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -4340,7 +4456,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -4354,7 +4470,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -4368,7 +4484,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>
@@ -4382,12 +4498,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="146" spans="6:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="6:10">
       <c r="F146" s="15" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="G146" s="15" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="H146" s="16" t="s">
         <v>1</v>
@@ -4399,12 +4515,12 @@
         <v>301</v>
       </c>
     </row>
-    <row r="147" spans="6:10" ht="54" x14ac:dyDescent="0.35">
-      <c r="F147" s="34" t="s">
+    <row r="147" spans="6:10" ht="54">
+      <c r="F147" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="G147" s="36" t="s">
-        <v>612</v>
+      <c r="G147" s="33" t="s">
+        <v>611</v>
       </c>
       <c r="H147" s="16" t="s">
         <v>299</v>
@@ -4416,10 +4532,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="148" spans="6:10" ht="54" x14ac:dyDescent="0.35">
-      <c r="F148" s="34"/>
-      <c r="G148" s="37" t="s">
-        <v>613</v>
+    <row r="148" spans="6:10" ht="54">
+      <c r="F148" s="46"/>
+      <c r="G148" s="34" t="s">
+        <v>612</v>
       </c>
       <c r="H148" s="16" t="s">
         <v>158</v>
@@ -4431,12 +4547,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="149" spans="6:10" ht="54" x14ac:dyDescent="0.35">
-      <c r="F149" s="34" t="s">
+    <row r="149" spans="6:10" ht="54">
+      <c r="F149" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="G149" s="36" t="s">
-        <v>612</v>
+      <c r="G149" s="33" t="s">
+        <v>611</v>
       </c>
       <c r="H149" s="16" t="s">
         <v>305</v>
@@ -4448,10 +4564,10 @@
         <v>560</v>
       </c>
     </row>
-    <row r="150" spans="6:10" ht="54" x14ac:dyDescent="0.35">
-      <c r="F150" s="34"/>
-      <c r="G150" s="37" t="s">
-        <v>613</v>
+    <row r="150" spans="6:10" ht="54">
+      <c r="F150" s="46"/>
+      <c r="G150" s="34" t="s">
+        <v>612</v>
       </c>
       <c r="H150" s="15" t="s">
         <v>189</v>
@@ -4463,12 +4579,12 @@
         <v>730</v>
       </c>
     </row>
-    <row r="151" spans="6:10" ht="54" x14ac:dyDescent="0.35">
-      <c r="F151" s="35" t="s">
+    <row r="151" spans="6:10" ht="54">
+      <c r="F151" s="46" t="s">
         <v>307</v>
       </c>
-      <c r="G151" s="36" t="s">
-        <v>612</v>
+      <c r="G151" s="33" t="s">
+        <v>611</v>
       </c>
       <c r="H151" s="16" t="s">
         <v>309</v>
@@ -4480,10 +4596,10 @@
         <v>112</v>
       </c>
     </row>
-    <row r="152" spans="6:10" ht="54" x14ac:dyDescent="0.35">
-      <c r="F152" s="35"/>
-      <c r="G152" s="37" t="s">
-        <v>613</v>
+    <row r="152" spans="6:10" ht="54">
+      <c r="F152" s="46"/>
+      <c r="G152" s="34" t="s">
+        <v>612</v>
       </c>
       <c r="H152" s="15" t="s">
         <v>226</v>
@@ -4495,12 +4611,12 @@
         <v>146</v>
       </c>
     </row>
-    <row r="153" spans="6:10" ht="54" x14ac:dyDescent="0.35">
-      <c r="F153" s="34" t="s">
+    <row r="153" spans="6:10" ht="54">
+      <c r="F153" s="46" t="s">
         <v>310</v>
       </c>
-      <c r="G153" s="36" t="s">
-        <v>612</v>
+      <c r="G153" s="33" t="s">
+        <v>611</v>
       </c>
       <c r="H153" s="16" t="s">
         <v>311</v>
@@ -4512,10 +4628,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="154" spans="6:10" ht="54" x14ac:dyDescent="0.35">
-      <c r="F154" s="34"/>
-      <c r="G154" s="37" t="s">
-        <v>613</v>
+    <row r="154" spans="6:10" ht="54">
+      <c r="F154" s="46"/>
+      <c r="G154" s="34" t="s">
+        <v>612</v>
       </c>
       <c r="H154" s="15" t="s">
         <v>253</v>
@@ -4527,7 +4643,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="194" ht="36" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="194" ht="36" customHeight="1"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="F147:F148"/>
@@ -4544,11 +4660,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A8515C-8539-4E5E-AB27-D793F52CD44C}">
   <dimension ref="A1:J142"/>
   <sheetViews>
-    <sheetView zoomScale="62" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="F61" zoomScale="50" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72:J77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="34.21875" style="4" bestFit="1" customWidth="1"/>
@@ -4562,7 +4678,7 @@
     <col min="11" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="54">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -4576,12 +4692,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="36">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -4595,7 +4711,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -4609,7 +4725,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -4624,13 +4740,13 @@
       </c>
       <c r="H5" s="25"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -4644,7 +4760,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -4658,7 +4774,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -4672,7 +4788,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -4686,7 +4802,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -4700,7 +4816,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -4714,13 +4830,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -4734,7 +4850,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -4748,7 +4864,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -4762,7 +4878,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -4776,7 +4892,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -4790,13 +4906,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -4810,7 +4926,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -4824,7 +4940,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -4838,13 +4954,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -4858,7 +4974,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -4872,7 +4988,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -4886,13 +5002,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -4906,7 +5022,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -4920,7 +5036,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -4934,13 +5050,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -4954,7 +5070,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -4968,7 +5084,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -4982,12 +5098,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -5001,7 +5117,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -5015,7 +5131,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -5029,13 +5145,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -5049,7 +5165,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -5063,7 +5179,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -5077,13 +5193,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -5097,7 +5213,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -5111,7 +5227,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -5125,12 +5241,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -5144,7 +5260,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -5158,7 +5274,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -5172,12 +5288,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -5191,7 +5307,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -5205,7 +5321,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -5219,12 +5335,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -5238,7 +5354,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -5252,7 +5368,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -5266,13 +5382,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -5286,7 +5402,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -5300,7 +5416,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -5314,13 +5430,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -5334,7 +5450,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -5348,7 +5464,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -5362,13 +5478,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -5382,7 +5498,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -5396,7 +5512,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -5410,12 +5526,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -5438,7 +5554,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -5461,7 +5577,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -5484,7 +5600,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -5507,7 +5623,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -5530,7 +5646,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5544,7 +5660,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -5561,7 +5677,7 @@
       <c r="I78" s="29"/>
       <c r="J78" s="29"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -5575,7 +5691,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -5589,7 +5705,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
@@ -5603,7 +5719,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -5617,11 +5733,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -5635,7 +5751,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -5649,7 +5765,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -5663,7 +5779,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -5677,7 +5793,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -5691,10 +5807,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -5708,7 +5824,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -5722,7 +5838,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -5736,7 +5852,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -5750,7 +5866,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -5764,10 +5880,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -5781,7 +5897,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -5795,7 +5911,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
@@ -5809,7 +5925,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -5823,7 +5939,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -5837,10 +5953,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -5854,7 +5970,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -5868,7 +5984,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -5882,7 +5998,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -5896,7 +6012,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -5910,10 +6026,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -5927,7 +6043,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -5941,7 +6057,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -5955,7 +6071,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -5969,7 +6085,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -5983,7 +6099,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -5997,7 +6113,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -6011,7 +6127,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -6025,7 +6141,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -6039,7 +6155,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -6053,7 +6169,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -6067,7 +6183,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -6081,7 +6197,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -6095,7 +6211,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -6109,7 +6225,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -6123,7 +6239,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -6137,7 +6253,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -6151,7 +6267,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
@@ -6165,7 +6281,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -6179,7 +6295,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -6193,7 +6309,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -6207,7 +6323,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
         <v>423</v>
       </c>
@@ -6221,7 +6337,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -6235,7 +6351,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
@@ -6249,7 +6365,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -6263,7 +6379,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -6277,7 +6393,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -6291,7 +6407,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -6305,7 +6421,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -6319,7 +6435,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>
@@ -6343,11 +6459,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF4B17E-1BBF-4C2E-9D6B-BC1E5266428F}">
   <dimension ref="A1:M142"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="66" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="E54" zoomScale="51" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="K71" sqref="K71:M76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="71" style="4" customWidth="1"/>
     <col min="2" max="2" width="34.21875" style="4" bestFit="1" customWidth="1"/>
@@ -6361,7 +6477,7 @@
     <col min="14" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="54" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="54">
       <c r="A1" s="5" t="s">
         <v>114</v>
       </c>
@@ -6375,12 +6491,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="36" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="36">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6394,7 +6510,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
         <v>89</v>
       </c>
@@ -6408,7 +6524,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -6422,13 +6538,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" s="2"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -6442,7 +6558,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
         <v>91</v>
       </c>
@@ -6456,7 +6572,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
         <v>92</v>
       </c>
@@ -6470,7 +6586,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
         <v>93</v>
       </c>
@@ -6484,7 +6600,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
         <v>94</v>
       </c>
@@ -6498,7 +6614,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
         <v>95</v>
       </c>
@@ -6512,13 +6628,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
         <v>96</v>
       </c>
@@ -6532,7 +6648,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>97</v>
       </c>
@@ -6546,7 +6662,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
         <v>98</v>
       </c>
@@ -6560,7 +6676,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -6574,7 +6690,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4">
       <c r="A18" s="2" t="s">
         <v>26</v>
       </c>
@@ -6588,13 +6704,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4">
       <c r="A20" s="2" t="s">
         <v>99</v>
       </c>
@@ -6608,7 +6724,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4">
       <c r="A21" s="2" t="s">
         <v>100</v>
       </c>
@@ -6622,7 +6738,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4">
       <c r="A22" s="2" t="s">
         <v>101</v>
       </c>
@@ -6636,13 +6752,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4">
       <c r="A24" s="2" t="s">
         <v>102</v>
       </c>
@@ -6656,7 +6772,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4">
       <c r="A25" s="2" t="s">
         <v>103</v>
       </c>
@@ -6670,7 +6786,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4">
       <c r="A26" s="2" t="s">
         <v>104</v>
       </c>
@@ -6684,13 +6800,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4">
       <c r="A28" s="2" t="s">
         <v>105</v>
       </c>
@@ -6704,7 +6820,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4">
       <c r="A29" s="2" t="s">
         <v>106</v>
       </c>
@@ -6718,7 +6834,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4">
       <c r="A30" s="2" t="s">
         <v>107</v>
       </c>
@@ -6732,13 +6848,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4">
       <c r="A32" s="2" t="s">
         <v>108</v>
       </c>
@@ -6752,7 +6868,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4">
       <c r="A33" s="2" t="s">
         <v>109</v>
       </c>
@@ -6766,7 +6882,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4">
       <c r="A34" s="2" t="s">
         <v>110</v>
       </c>
@@ -6780,12 +6896,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4">
       <c r="A36" s="2" t="s">
         <v>111</v>
       </c>
@@ -6799,7 +6915,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4">
       <c r="A37" s="2" t="s">
         <v>112</v>
       </c>
@@ -6813,7 +6929,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -6827,13 +6943,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4">
       <c r="A39" s="2"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4">
       <c r="A40" s="2" t="s">
         <v>5</v>
       </c>
@@ -6847,7 +6963,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4">
       <c r="A41" s="2" t="s">
         <v>9</v>
       </c>
@@ -6861,7 +6977,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -6875,13 +6991,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4">
       <c r="A43" s="2"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4">
       <c r="A44" s="2" t="s">
         <v>6</v>
       </c>
@@ -6895,7 +7011,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -6909,7 +7025,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -6923,12 +7039,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4">
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4">
       <c r="A48" s="2" t="s">
         <v>7</v>
       </c>
@@ -6942,7 +7058,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4">
       <c r="A49" s="2" t="s">
         <v>11</v>
       </c>
@@ -6956,7 +7072,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4">
       <c r="A50" s="2" t="s">
         <v>15</v>
       </c>
@@ -6970,12 +7086,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4">
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4">
       <c r="A52" s="2" t="s">
         <v>8</v>
       </c>
@@ -6989,7 +7105,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4">
       <c r="A53" s="2" t="s">
         <v>12</v>
       </c>
@@ -7003,7 +7119,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4">
       <c r="A54" s="2" t="s">
         <v>16</v>
       </c>
@@ -7017,12 +7133,12 @@
         <v>116</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4">
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4">
       <c r="A56" s="2" t="s">
         <v>27</v>
       </c>
@@ -7036,7 +7152,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4">
       <c r="A57" s="2" t="s">
         <v>28</v>
       </c>
@@ -7050,7 +7166,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4">
       <c r="A58" s="2" t="s">
         <v>29</v>
       </c>
@@ -7064,13 +7180,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4">
       <c r="A59" s="2"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -7084,7 +7200,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4">
       <c r="A61" s="2" t="s">
         <v>31</v>
       </c>
@@ -7098,7 +7214,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4">
       <c r="A62" s="2" t="s">
         <v>32</v>
       </c>
@@ -7112,13 +7228,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4">
       <c r="A63" s="2"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4">
       <c r="A64" s="2" t="s">
         <v>33</v>
       </c>
@@ -7132,7 +7248,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:13">
       <c r="A65" s="2" t="s">
         <v>34</v>
       </c>
@@ -7146,7 +7262,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:13">
       <c r="A66" s="2" t="s">
         <v>35</v>
       </c>
@@ -7160,13 +7276,13 @@
         <v>116</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:13">
       <c r="A67" s="2"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:13">
       <c r="A68" s="2" t="s">
         <v>36</v>
       </c>
@@ -7180,7 +7296,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:13">
       <c r="A69" s="2" t="s">
         <v>37</v>
       </c>
@@ -7194,7 +7310,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:13">
       <c r="A70" s="2" t="s">
         <v>38</v>
       </c>
@@ -7208,7 +7324,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:13">
       <c r="A71" s="2"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -7222,7 +7338,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:13">
       <c r="A72" s="2" t="s">
         <v>17</v>
       </c>
@@ -7245,7 +7361,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:13">
       <c r="A73" s="2" t="s">
         <v>18</v>
       </c>
@@ -7258,7 +7374,7 @@
       <c r="D73" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="K73" s="33" t="s">
+      <c r="K73" s="32" t="s">
         <v>605</v>
       </c>
       <c r="L73" s="3" t="s">
@@ -7268,7 +7384,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:13">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -7281,7 +7397,7 @@
       <c r="D74" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="K74" s="33" t="s">
+      <c r="K74" s="32" t="s">
         <v>610</v>
       </c>
       <c r="L74" s="4" t="s">
@@ -7291,7 +7407,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:13">
       <c r="A75" s="2" t="s">
         <v>39</v>
       </c>
@@ -7314,7 +7430,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:13">
       <c r="A76" s="2" t="s">
         <v>40</v>
       </c>
@@ -7337,12 +7453,12 @@
         <v>580</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:13">
       <c r="A77" s="2"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:13">
       <c r="A78" s="2" t="s">
         <v>20</v>
       </c>
@@ -7356,7 +7472,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:13">
       <c r="A79" s="4" t="s">
         <v>21</v>
       </c>
@@ -7370,7 +7486,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:13">
       <c r="A80" s="2" t="s">
         <v>22</v>
       </c>
@@ -7384,7 +7500,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4">
       <c r="A81" s="2" t="s">
         <v>41</v>
       </c>
@@ -7398,7 +7514,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:4">
       <c r="A82" s="2" t="s">
         <v>42</v>
       </c>
@@ -7412,11 +7528,11 @@
         <v>144</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:4">
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:4">
       <c r="A84" s="2" t="s">
         <v>23</v>
       </c>
@@ -7430,7 +7546,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:4">
       <c r="A85" s="2" t="s">
         <v>24</v>
       </c>
@@ -7444,7 +7560,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:4">
       <c r="A86" s="2" t="s">
         <v>25</v>
       </c>
@@ -7458,7 +7574,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:4">
       <c r="A87" s="2" t="s">
         <v>43</v>
       </c>
@@ -7472,7 +7588,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:4">
       <c r="A88" s="2" t="s">
         <v>44</v>
       </c>
@@ -7486,10 +7602,10 @@
         <v>144</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:4">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:4">
       <c r="A90" s="2" t="s">
         <v>45</v>
       </c>
@@ -7503,7 +7619,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:4">
       <c r="A91" s="2" t="s">
         <v>46</v>
       </c>
@@ -7517,7 +7633,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:4">
       <c r="A92" s="2" t="s">
         <v>47</v>
       </c>
@@ -7531,7 +7647,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:4">
       <c r="A93" s="2" t="s">
         <v>48</v>
       </c>
@@ -7545,7 +7661,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4">
       <c r="A94" s="2" t="s">
         <v>49</v>
       </c>
@@ -7559,10 +7675,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:4">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:4">
       <c r="A96" s="2" t="s">
         <v>50</v>
       </c>
@@ -7576,7 +7692,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:4">
       <c r="A97" s="2" t="s">
         <v>51</v>
       </c>
@@ -7590,7 +7706,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:4">
       <c r="A98" s="2" t="s">
         <v>52</v>
       </c>
@@ -7604,7 +7720,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:4">
       <c r="A99" s="2" t="s">
         <v>53</v>
       </c>
@@ -7618,7 +7734,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:4">
       <c r="A100" s="2" t="s">
         <v>54</v>
       </c>
@@ -7632,10 +7748,10 @@
         <v>175</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:4">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:4">
       <c r="A102" s="2" t="s">
         <v>55</v>
       </c>
@@ -7649,7 +7765,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:4">
       <c r="A103" s="2" t="s">
         <v>56</v>
       </c>
@@ -7663,7 +7779,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:4">
       <c r="A104" s="2" t="s">
         <v>57</v>
       </c>
@@ -7677,7 +7793,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:4">
       <c r="A105" s="2" t="s">
         <v>58</v>
       </c>
@@ -7691,7 +7807,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:4">
       <c r="A106" s="2" t="s">
         <v>59</v>
       </c>
@@ -7705,10 +7821,10 @@
         <v>191</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:4">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:4">
       <c r="A108" s="2" t="s">
         <v>60</v>
       </c>
@@ -7722,7 +7838,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:4">
       <c r="A109" s="2" t="s">
         <v>61</v>
       </c>
@@ -7736,7 +7852,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
         <v>62</v>
       </c>
@@ -7750,7 +7866,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:4">
       <c r="A111" s="4" t="s">
         <v>63</v>
       </c>
@@ -7764,7 +7880,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:4">
       <c r="A112" s="4" t="s">
         <v>64</v>
       </c>
@@ -7778,7 +7894,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:4">
       <c r="A114" s="4" t="s">
         <v>65</v>
       </c>
@@ -7792,7 +7908,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:4">
       <c r="A115" s="4" t="s">
         <v>219</v>
       </c>
@@ -7806,7 +7922,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:4">
       <c r="A116" s="4" t="s">
         <v>66</v>
       </c>
@@ -7820,7 +7936,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:4">
       <c r="A117" s="4" t="s">
         <v>67</v>
       </c>
@@ -7834,7 +7950,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:4">
       <c r="A118" s="4" t="s">
         <v>68</v>
       </c>
@@ -7848,7 +7964,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:4">
       <c r="A120" s="4" t="s">
         <v>69</v>
       </c>
@@ -7862,7 +7978,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:4">
       <c r="A121" s="4" t="s">
         <v>70</v>
       </c>
@@ -7876,7 +7992,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:4">
       <c r="A122" s="4" t="s">
         <v>71</v>
       </c>
@@ -7890,7 +8006,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:4">
       <c r="A123" s="4" t="s">
         <v>72</v>
       </c>
@@ -7904,7 +8020,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:4">
       <c r="A124" s="4" t="s">
         <v>73</v>
       </c>
@@ -7918,7 +8034,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:4">
       <c r="A126" s="4" t="s">
         <v>74</v>
       </c>
@@ -7932,7 +8048,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:4">
       <c r="A127" s="4" t="s">
         <v>75</v>
       </c>
@@ -7946,7 +8062,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:4">
       <c r="A128" s="4" t="s">
         <v>76</v>
       </c>
@@ -7960,7 +8076,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:4">
       <c r="A129" s="4" t="s">
         <v>77</v>
       </c>
@@ -7974,7 +8090,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:4">
       <c r="A130" s="4" t="s">
         <v>78</v>
       </c>
@@ -7988,7 +8104,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:4">
       <c r="A132" s="4" t="s">
         <v>79</v>
       </c>
@@ -8002,7 +8118,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:4">
       <c r="A133" s="4" t="s">
         <v>80</v>
       </c>
@@ -8016,7 +8132,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:4">
       <c r="A134" s="4" t="s">
         <v>81</v>
       </c>
@@ -8030,7 +8146,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:4">
       <c r="A135" s="4" t="s">
         <v>82</v>
       </c>
@@ -8044,7 +8160,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:4">
       <c r="A136" s="4" t="s">
         <v>83</v>
       </c>
@@ -8058,7 +8174,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:4">
       <c r="A138" s="4" t="s">
         <v>84</v>
       </c>
@@ -8072,7 +8188,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:4">
       <c r="A139" s="4" t="s">
         <v>85</v>
       </c>
@@ -8086,7 +8202,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:4">
       <c r="A140" s="4" t="s">
         <v>86</v>
       </c>
@@ -8100,7 +8216,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:4">
       <c r="A141" s="4" t="s">
         <v>87</v>
       </c>
@@ -8114,7 +8230,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:4">
       <c r="A142" s="4" t="s">
         <v>88</v>
       </c>

</xml_diff>